<commit_message>
final draft of notebook
</commit_message>
<xml_diff>
--- a/Data/spending.xlsx
+++ b/Data/spending.xlsx
@@ -11,6 +11,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20231" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20232" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20233" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20234" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -15908,6 +15909,798 @@
       </c>
     </row>
     <row r="3">
+      <c r="A3" s="5" t="n"/>
+      <c r="B3" s="4" t="inlineStr">
+        <is>
+          <t>Counter</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>-44.16</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-60.93</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-24</v>
+      </c>
+      <c r="G3" t="n">
+        <v>-69.73</v>
+      </c>
+      <c r="H3" t="n">
+        <v>-44.56999999999999</v>
+      </c>
+      <c r="I3" t="n">
+        <v>-28.27</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>-3.54</v>
+      </c>
+      <c r="L3" t="n">
+        <v>-48.43</v>
+      </c>
+      <c r="M3" t="n">
+        <v>-11.84</v>
+      </c>
+      <c r="N3" t="n">
+        <v>-4.35</v>
+      </c>
+      <c r="O3" t="n">
+        <v>-339.82</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="inlineStr">
+        <is>
+          <t>Food</t>
+        </is>
+      </c>
+      <c r="B4" s="4" t="inlineStr">
+        <is>
+          <t>Groceries</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>-6.67</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-14.48</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-61.58</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>-20.82</v>
+      </c>
+      <c r="H4" t="n">
+        <v>-68.91</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>-7.42</v>
+      </c>
+      <c r="L4" t="n">
+        <v>-2.49</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>-15.99</v>
+      </c>
+      <c r="O4" t="n">
+        <v>-198.36</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="n"/>
+      <c r="B5" s="4" t="inlineStr">
+        <is>
+          <t>Restaurant</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>-54.54</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-19.77</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-19.07</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-56.84999999999999</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-188.11</v>
+      </c>
+      <c r="H5" t="n">
+        <v>-124.51</v>
+      </c>
+      <c r="I5" t="n">
+        <v>-66.7</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>-109.59</v>
+      </c>
+      <c r="L5" t="n">
+        <v>-80.69</v>
+      </c>
+      <c r="M5" t="n">
+        <v>-68.73</v>
+      </c>
+      <c r="N5" t="n">
+        <v>-63.09</v>
+      </c>
+      <c r="O5" t="n">
+        <v>-851.6500000000002</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="inlineStr">
+        <is>
+          <t>Income</t>
+        </is>
+      </c>
+      <c r="B6" s="4" t="inlineStr">
+        <is>
+          <t>Tutoring</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>348.44</v>
+      </c>
+      <c r="M6" t="n">
+        <v>962.03</v>
+      </c>
+      <c r="N6" t="n">
+        <v>694.49</v>
+      </c>
+      <c r="O6" t="n">
+        <v>2004.96</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="inlineStr">
+        <is>
+          <t>Miscellaneous</t>
+        </is>
+      </c>
+      <c r="B7" s="4" t="inlineStr">
+        <is>
+          <t>Bank</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>-199.67</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-19.86</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-18.92</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-58.89</v>
+      </c>
+      <c r="G7" t="n">
+        <v>-38.91</v>
+      </c>
+      <c r="H7" t="n">
+        <v>-79.24000000000001</v>
+      </c>
+      <c r="I7" t="n">
+        <v>-59.25</v>
+      </c>
+      <c r="J7" t="n">
+        <v>-39.24</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="M7" t="n">
+        <v>-59.9</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" t="n">
+        <v>-573.4400000000001</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="5" t="n"/>
+      <c r="B8" s="4" t="inlineStr">
+        <is>
+          <t>Miscellaneous</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>-106.48</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-74.8</v>
+      </c>
+      <c r="E8" t="n">
+        <v>3476.46</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-146.88</v>
+      </c>
+      <c r="G8" t="n">
+        <v>-173.02</v>
+      </c>
+      <c r="H8" t="n">
+        <v>94.92</v>
+      </c>
+      <c r="I8" t="n">
+        <v>349.8</v>
+      </c>
+      <c r="J8" t="n">
+        <v>-66.71000000000001</v>
+      </c>
+      <c r="K8" t="n">
+        <v>-187.81</v>
+      </c>
+      <c r="L8" t="n">
+        <v>-57.46000000000001</v>
+      </c>
+      <c r="M8" t="n">
+        <v>-234.09</v>
+      </c>
+      <c r="N8" t="n">
+        <v>-166.94</v>
+      </c>
+      <c r="O8" t="n">
+        <v>2706.99</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="inlineStr">
+        <is>
+          <t>Pharmacy</t>
+        </is>
+      </c>
+      <c r="B9" s="4" t="inlineStr">
+        <is>
+          <t>Pharmacy</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>-2.54</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-15.95</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-22.92</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-29.58</v>
+      </c>
+      <c r="G9" t="n">
+        <v>-53.01</v>
+      </c>
+      <c r="H9" t="n">
+        <v>-5.99</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>-6.99</v>
+      </c>
+      <c r="L9" t="n">
+        <v>-5.84</v>
+      </c>
+      <c r="M9" t="n">
+        <v>-25.06</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" t="n">
+        <v>-167.88</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="inlineStr">
+        <is>
+          <t>Rent</t>
+        </is>
+      </c>
+      <c r="B10" s="4" t="inlineStr">
+        <is>
+          <t>Rent</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="inlineStr">
+        <is>
+          <t>Savings</t>
+        </is>
+      </c>
+      <c r="B11" s="4" t="inlineStr">
+        <is>
+          <t>Savings</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>-1000</v>
+      </c>
+      <c r="L11" t="n">
+        <v>-250</v>
+      </c>
+      <c r="M11" t="n">
+        <v>-649.23</v>
+      </c>
+      <c r="N11" t="n">
+        <v>-499.32</v>
+      </c>
+      <c r="O11" t="n">
+        <v>-2398.55</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="inlineStr">
+        <is>
+          <t>Transportation</t>
+        </is>
+      </c>
+      <c r="B12" s="4" t="inlineStr">
+        <is>
+          <t>Parking</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-15</v>
+      </c>
+      <c r="F12" t="n">
+        <v>-4.25</v>
+      </c>
+      <c r="G12" t="n">
+        <v>-4</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" t="n">
+        <v>-23.25</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="6" t="n"/>
+      <c r="B13" s="4" t="inlineStr">
+        <is>
+          <t>Plane</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>-150</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>-30</v>
+      </c>
+      <c r="O13" t="n">
+        <v>-180</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="6" t="n"/>
+      <c r="B14" s="4" t="inlineStr">
+        <is>
+          <t>Rideshare</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>0</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-31.26</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-67.8</v>
+      </c>
+      <c r="G14" t="n">
+        <v>-182.1</v>
+      </c>
+      <c r="H14" t="n">
+        <v>-59.73</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" t="n">
+        <v>-70.12</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" t="n">
+        <v>-411.01</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="5" t="n"/>
+      <c r="B15" s="4" t="inlineStr">
+        <is>
+          <t>Train</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>-72</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-31</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" t="n">
+        <v>-103</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A12:A15"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:O15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Category</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>Subcategory</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>January</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>February</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>March</t>
+        </is>
+      </c>
+      <c r="F1" s="4" t="inlineStr">
+        <is>
+          <t>April</t>
+        </is>
+      </c>
+      <c r="G1" s="4" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+      <c r="H1" s="4" t="inlineStr">
+        <is>
+          <t>June</t>
+        </is>
+      </c>
+      <c r="I1" s="4" t="inlineStr">
+        <is>
+          <t>July</t>
+        </is>
+      </c>
+      <c r="J1" s="4" t="inlineStr">
+        <is>
+          <t>August</t>
+        </is>
+      </c>
+      <c r="K1" s="4" t="inlineStr">
+        <is>
+          <t>September</t>
+        </is>
+      </c>
+      <c r="L1" s="4" t="inlineStr">
+        <is>
+          <t>October</t>
+        </is>
+      </c>
+      <c r="M1" s="4" t="inlineStr">
+        <is>
+          <t>November</t>
+        </is>
+      </c>
+      <c r="N1" s="4" t="inlineStr">
+        <is>
+          <t>December</t>
+        </is>
+      </c>
+      <c r="O1" s="4" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="inlineStr">
+        <is>
+          <t>Drink</t>
+        </is>
+      </c>
+      <c r="B2" s="4" t="inlineStr">
+        <is>
+          <t>Bar</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-39.53</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-37.69</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
+      </c>
+      <c r="H2" t="n">
+        <v>-36.58</v>
+      </c>
+      <c r="I2" t="n">
+        <v>-23.2</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>-52.1</v>
+      </c>
+      <c r="L2" t="n">
+        <v>-30.94</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0</v>
+      </c>
+      <c r="O2" t="n">
+        <v>-220.04</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" s="4" t="n"/>
       <c r="B3" s="4" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
test images in readme
</commit_message>
<xml_diff>
--- a/Data/spending.xlsx
+++ b/Data/spending.xlsx
@@ -7,11 +7,7 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="original" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20231" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20232" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20233" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="20234" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023_spending" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -82,7 +78,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -90,8 +86,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -13345,849 +13339,6 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O16"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="4" t="inlineStr">
-        <is>
-          <t>Category</t>
-        </is>
-      </c>
-      <c r="B1" s="4" t="inlineStr">
-        <is>
-          <t>Subcategory</t>
-        </is>
-      </c>
-      <c r="C1" s="4" t="inlineStr">
-        <is>
-          <t>January</t>
-        </is>
-      </c>
-      <c r="D1" s="4" t="inlineStr">
-        <is>
-          <t>February</t>
-        </is>
-      </c>
-      <c r="E1" s="4" t="inlineStr">
-        <is>
-          <t>March</t>
-        </is>
-      </c>
-      <c r="F1" s="4" t="inlineStr">
-        <is>
-          <t>April</t>
-        </is>
-      </c>
-      <c r="G1" s="4" t="inlineStr">
-        <is>
-          <t>May</t>
-        </is>
-      </c>
-      <c r="H1" s="4" t="inlineStr">
-        <is>
-          <t>June</t>
-        </is>
-      </c>
-      <c r="I1" s="4" t="inlineStr">
-        <is>
-          <t>July</t>
-        </is>
-      </c>
-      <c r="J1" s="4" t="inlineStr">
-        <is>
-          <t>August</t>
-        </is>
-      </c>
-      <c r="K1" s="4" t="inlineStr">
-        <is>
-          <t>September</t>
-        </is>
-      </c>
-      <c r="L1" s="4" t="inlineStr">
-        <is>
-          <t>October</t>
-        </is>
-      </c>
-      <c r="M1" s="4" t="inlineStr">
-        <is>
-          <t>November</t>
-        </is>
-      </c>
-      <c r="N1" s="4" t="inlineStr">
-        <is>
-          <t>December</t>
-        </is>
-      </c>
-      <c r="O1" s="4" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="inlineStr">
-        <is>
-          <t>Drink</t>
-        </is>
-      </c>
-      <c r="B2" s="4" t="inlineStr">
-        <is>
-          <t>Bar</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>-39.53</v>
-      </c>
-      <c r="F2" t="n">
-        <v>-37.69</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>-36.58</v>
-      </c>
-      <c r="I2" t="n">
-        <v>-23.2</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" t="n">
-        <v>-52.1</v>
-      </c>
-      <c r="L2" t="n">
-        <v>-30.94</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" t="n">
-        <v>-220.04</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="5" t="n"/>
-      <c r="B3" s="4" t="inlineStr">
-        <is>
-          <t>Counter</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>-44.16</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>-60.93</v>
-      </c>
-      <c r="F3" t="n">
-        <v>-24</v>
-      </c>
-      <c r="G3" t="n">
-        <v>-69.73</v>
-      </c>
-      <c r="H3" t="n">
-        <v>-44.56999999999999</v>
-      </c>
-      <c r="I3" t="n">
-        <v>-28.27</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" t="n">
-        <v>-3.54</v>
-      </c>
-      <c r="L3" t="n">
-        <v>-48.43</v>
-      </c>
-      <c r="M3" t="n">
-        <v>-11.84</v>
-      </c>
-      <c r="N3" t="n">
-        <v>-4.35</v>
-      </c>
-      <c r="O3" t="n">
-        <v>-339.82</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="inlineStr">
-        <is>
-          <t>Food</t>
-        </is>
-      </c>
-      <c r="B4" s="4" t="inlineStr">
-        <is>
-          <t>Groceries</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>-6.67</v>
-      </c>
-      <c r="D4" t="n">
-        <v>-14.48</v>
-      </c>
-      <c r="E4" t="n">
-        <v>-61.58</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>-20.82</v>
-      </c>
-      <c r="H4" t="n">
-        <v>-68.91</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" t="n">
-        <v>-7.42</v>
-      </c>
-      <c r="L4" t="n">
-        <v>-2.49</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" t="n">
-        <v>-15.99</v>
-      </c>
-      <c r="O4" t="n">
-        <v>-198.36</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="n"/>
-      <c r="B5" s="4" t="inlineStr">
-        <is>
-          <t>Restaurant</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>-54.54</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-19.77</v>
-      </c>
-      <c r="E5" t="n">
-        <v>-19.07</v>
-      </c>
-      <c r="F5" t="n">
-        <v>-56.84999999999999</v>
-      </c>
-      <c r="G5" t="n">
-        <v>-188.11</v>
-      </c>
-      <c r="H5" t="n">
-        <v>-124.51</v>
-      </c>
-      <c r="I5" t="n">
-        <v>-66.7</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" t="n">
-        <v>-109.59</v>
-      </c>
-      <c r="L5" t="n">
-        <v>-80.69</v>
-      </c>
-      <c r="M5" t="n">
-        <v>-68.73</v>
-      </c>
-      <c r="N5" t="n">
-        <v>-63.09</v>
-      </c>
-      <c r="O5" t="n">
-        <v>-851.6500000000002</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="inlineStr">
-        <is>
-          <t>Income</t>
-        </is>
-      </c>
-      <c r="B6" s="4" t="inlineStr">
-        <is>
-          <t>Tutoring</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L6" t="n">
-        <v>348.44</v>
-      </c>
-      <c r="M6" t="n">
-        <v>962.03</v>
-      </c>
-      <c r="N6" t="n">
-        <v>694.49</v>
-      </c>
-      <c r="O6" t="n">
-        <v>2004.96</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="inlineStr">
-        <is>
-          <t>Miscellaneous</t>
-        </is>
-      </c>
-      <c r="B7" s="4" t="inlineStr">
-        <is>
-          <t>Bank</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>-199.67</v>
-      </c>
-      <c r="D7" t="n">
-        <v>-19.86</v>
-      </c>
-      <c r="E7" t="n">
-        <v>-18.92</v>
-      </c>
-      <c r="F7" t="n">
-        <v>-58.89</v>
-      </c>
-      <c r="G7" t="n">
-        <v>-38.91</v>
-      </c>
-      <c r="H7" t="n">
-        <v>-79.24000000000001</v>
-      </c>
-      <c r="I7" t="n">
-        <v>-59.25</v>
-      </c>
-      <c r="J7" t="n">
-        <v>-39.24</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="M7" t="n">
-        <v>-59.9</v>
-      </c>
-      <c r="N7" t="n">
-        <v>0</v>
-      </c>
-      <c r="O7" t="n">
-        <v>-573.4400000000001</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="5" t="n"/>
-      <c r="B8" s="4" t="inlineStr">
-        <is>
-          <t>Miscellaneous</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0</v>
-      </c>
-      <c r="N8" t="n">
-        <v>0</v>
-      </c>
-      <c r="O8" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="4" t="inlineStr">
-        <is>
-          <t>Pharmacy</t>
-        </is>
-      </c>
-      <c r="B9" s="4" t="inlineStr">
-        <is>
-          <t>Pharmacy</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>-2.54</v>
-      </c>
-      <c r="D9" t="n">
-        <v>-15.95</v>
-      </c>
-      <c r="E9" t="n">
-        <v>-22.92</v>
-      </c>
-      <c r="F9" t="n">
-        <v>-29.58</v>
-      </c>
-      <c r="G9" t="n">
-        <v>-53.01</v>
-      </c>
-      <c r="H9" t="n">
-        <v>-5.99</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" t="n">
-        <v>-6.99</v>
-      </c>
-      <c r="L9" t="n">
-        <v>-5.84</v>
-      </c>
-      <c r="M9" t="n">
-        <v>-25.06</v>
-      </c>
-      <c r="N9" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" t="n">
-        <v>-167.88</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="4" t="inlineStr">
-        <is>
-          <t>Rent</t>
-        </is>
-      </c>
-      <c r="B10" s="4" t="inlineStr">
-        <is>
-          <t>Rent</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" t="n">
-        <v>0</v>
-      </c>
-      <c r="N10" t="n">
-        <v>0</v>
-      </c>
-      <c r="O10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="4" t="inlineStr">
-        <is>
-          <t>Savings</t>
-        </is>
-      </c>
-      <c r="B11" s="4" t="inlineStr">
-        <is>
-          <t>Savings</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0</v>
-      </c>
-      <c r="K11" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="L11" t="n">
-        <v>-250</v>
-      </c>
-      <c r="M11" t="n">
-        <v>-649.23</v>
-      </c>
-      <c r="N11" t="n">
-        <v>-499.32</v>
-      </c>
-      <c r="O11" t="n">
-        <v>-2398.55</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="4" t="inlineStr">
-        <is>
-          <t>Transportation</t>
-        </is>
-      </c>
-      <c r="B12" s="4" t="inlineStr">
-        <is>
-          <t>Parking</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" t="n">
-        <v>-15</v>
-      </c>
-      <c r="F12" t="n">
-        <v>-4.25</v>
-      </c>
-      <c r="G12" t="n">
-        <v>-4</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0</v>
-      </c>
-      <c r="K12" t="n">
-        <v>0</v>
-      </c>
-      <c r="L12" t="n">
-        <v>0</v>
-      </c>
-      <c r="M12" t="n">
-        <v>0</v>
-      </c>
-      <c r="N12" t="n">
-        <v>0</v>
-      </c>
-      <c r="O12" t="n">
-        <v>-23.25</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="6" t="n"/>
-      <c r="B13" s="4" t="inlineStr">
-        <is>
-          <t>Plane</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" t="n">
-        <v>-150</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" t="n">
-        <v>0</v>
-      </c>
-      <c r="K13" t="n">
-        <v>0</v>
-      </c>
-      <c r="L13" t="n">
-        <v>0</v>
-      </c>
-      <c r="M13" t="n">
-        <v>0</v>
-      </c>
-      <c r="N13" t="n">
-        <v>-30</v>
-      </c>
-      <c r="O13" t="n">
-        <v>-180</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="6" t="n"/>
-      <c r="B14" s="4" t="inlineStr">
-        <is>
-          <t>Rideshare</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" t="n">
-        <v>-31.26</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" t="n">
-        <v>-67.8</v>
-      </c>
-      <c r="G14" t="n">
-        <v>-182.1</v>
-      </c>
-      <c r="H14" t="n">
-        <v>-59.73</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" t="n">
-        <v>0</v>
-      </c>
-      <c r="K14" t="n">
-        <v>-70.12</v>
-      </c>
-      <c r="L14" t="n">
-        <v>0</v>
-      </c>
-      <c r="M14" t="n">
-        <v>0</v>
-      </c>
-      <c r="N14" t="n">
-        <v>0</v>
-      </c>
-      <c r="O14" t="n">
-        <v>-411.01</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="5" t="n"/>
-      <c r="B15" s="4" t="inlineStr">
-        <is>
-          <t>Train</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" t="n">
-        <v>-72</v>
-      </c>
-      <c r="E15" t="n">
-        <v>-31</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0</v>
-      </c>
-      <c r="G15" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" t="n">
-        <v>0</v>
-      </c>
-      <c r="K15" t="n">
-        <v>0</v>
-      </c>
-      <c r="L15" t="n">
-        <v>0</v>
-      </c>
-      <c r="M15" t="n">
-        <v>0</v>
-      </c>
-      <c r="N15" t="n">
-        <v>0</v>
-      </c>
-      <c r="O15" t="n">
-        <v>-103</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="4" t="inlineStr">
-        <is>
-          <t>miscellaneous</t>
-        </is>
-      </c>
-      <c r="B16" s="4" t="inlineStr">
-        <is>
-          <t>Miscellaneous</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>-106.48</v>
-      </c>
-      <c r="D16" t="n">
-        <v>-74.8</v>
-      </c>
-      <c r="E16" t="n">
-        <v>3476.46</v>
-      </c>
-      <c r="F16" t="n">
-        <v>-146.88</v>
-      </c>
-      <c r="G16" t="n">
-        <v>-173.02</v>
-      </c>
-      <c r="H16" t="n">
-        <v>94.92</v>
-      </c>
-      <c r="I16" t="n">
-        <v>349.8</v>
-      </c>
-      <c r="J16" t="n">
-        <v>-66.71000000000001</v>
-      </c>
-      <c r="K16" t="n">
-        <v>-187.81</v>
-      </c>
-      <c r="L16" t="n">
-        <v>-57.46000000000001</v>
-      </c>
-      <c r="M16" t="n">
-        <v>-234.09</v>
-      </c>
-      <c r="N16" t="n">
-        <v>-166.94</v>
-      </c>
-      <c r="O16" t="n">
-        <v>2706.99</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A12:A15"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -14325,2382 +13476,6 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="n"/>
-      <c r="B3" s="4" t="inlineStr">
-        <is>
-          <t>Counter</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>-44.16</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>-60.93</v>
-      </c>
-      <c r="F3" t="n">
-        <v>-24</v>
-      </c>
-      <c r="G3" t="n">
-        <v>-69.73</v>
-      </c>
-      <c r="H3" t="n">
-        <v>-44.56999999999999</v>
-      </c>
-      <c r="I3" t="n">
-        <v>-28.27</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" t="n">
-        <v>-3.54</v>
-      </c>
-      <c r="L3" t="n">
-        <v>-48.43</v>
-      </c>
-      <c r="M3" t="n">
-        <v>-11.84</v>
-      </c>
-      <c r="N3" t="n">
-        <v>-4.35</v>
-      </c>
-      <c r="O3" t="n">
-        <v>-339.82</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="inlineStr">
-        <is>
-          <t>Food</t>
-        </is>
-      </c>
-      <c r="B4" s="4" t="inlineStr">
-        <is>
-          <t>Groceries</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>-6.67</v>
-      </c>
-      <c r="D4" t="n">
-        <v>-14.48</v>
-      </c>
-      <c r="E4" t="n">
-        <v>-61.58</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>-20.82</v>
-      </c>
-      <c r="H4" t="n">
-        <v>-68.91</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" t="n">
-        <v>-7.42</v>
-      </c>
-      <c r="L4" t="n">
-        <v>-2.49</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" t="n">
-        <v>-15.99</v>
-      </c>
-      <c r="O4" t="n">
-        <v>-198.36</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="n"/>
-      <c r="B5" s="4" t="inlineStr">
-        <is>
-          <t>Restaurant</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>-54.54</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-19.77</v>
-      </c>
-      <c r="E5" t="n">
-        <v>-19.07</v>
-      </c>
-      <c r="F5" t="n">
-        <v>-56.84999999999999</v>
-      </c>
-      <c r="G5" t="n">
-        <v>-188.11</v>
-      </c>
-      <c r="H5" t="n">
-        <v>-124.51</v>
-      </c>
-      <c r="I5" t="n">
-        <v>-66.7</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" t="n">
-        <v>-109.59</v>
-      </c>
-      <c r="L5" t="n">
-        <v>-80.69</v>
-      </c>
-      <c r="M5" t="n">
-        <v>-68.73</v>
-      </c>
-      <c r="N5" t="n">
-        <v>-63.09</v>
-      </c>
-      <c r="O5" t="n">
-        <v>-851.6500000000002</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="inlineStr">
-        <is>
-          <t>Income</t>
-        </is>
-      </c>
-      <c r="B6" s="4" t="inlineStr">
-        <is>
-          <t>Tutoring</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L6" t="n">
-        <v>348.44</v>
-      </c>
-      <c r="M6" t="n">
-        <v>962.03</v>
-      </c>
-      <c r="N6" t="n">
-        <v>694.49</v>
-      </c>
-      <c r="O6" t="n">
-        <v>2004.96</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="inlineStr">
-        <is>
-          <t>Miscellaneous</t>
-        </is>
-      </c>
-      <c r="B7" s="4" t="inlineStr">
-        <is>
-          <t>Bank</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>-199.67</v>
-      </c>
-      <c r="D7" t="n">
-        <v>-19.86</v>
-      </c>
-      <c r="E7" t="n">
-        <v>-18.92</v>
-      </c>
-      <c r="F7" t="n">
-        <v>-58.89</v>
-      </c>
-      <c r="G7" t="n">
-        <v>-38.91</v>
-      </c>
-      <c r="H7" t="n">
-        <v>-79.24000000000001</v>
-      </c>
-      <c r="I7" t="n">
-        <v>-59.25</v>
-      </c>
-      <c r="J7" t="n">
-        <v>-39.24</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="M7" t="n">
-        <v>-59.9</v>
-      </c>
-      <c r="N7" t="n">
-        <v>0</v>
-      </c>
-      <c r="O7" t="n">
-        <v>-573.4400000000001</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="5" t="n"/>
-      <c r="B8" s="4" t="inlineStr">
-        <is>
-          <t>Miscellaneous</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>-106.48</v>
-      </c>
-      <c r="D8" t="n">
-        <v>-74.8</v>
-      </c>
-      <c r="E8" t="n">
-        <v>3476.46</v>
-      </c>
-      <c r="F8" t="n">
-        <v>-146.88</v>
-      </c>
-      <c r="G8" t="n">
-        <v>-173.02</v>
-      </c>
-      <c r="H8" t="n">
-        <v>94.92</v>
-      </c>
-      <c r="I8" t="n">
-        <v>349.8</v>
-      </c>
-      <c r="J8" t="n">
-        <v>-66.71000000000001</v>
-      </c>
-      <c r="K8" t="n">
-        <v>-187.81</v>
-      </c>
-      <c r="L8" t="n">
-        <v>-57.46000000000001</v>
-      </c>
-      <c r="M8" t="n">
-        <v>-234.09</v>
-      </c>
-      <c r="N8" t="n">
-        <v>-166.94</v>
-      </c>
-      <c r="O8" t="n">
-        <v>2706.99</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="4" t="inlineStr">
-        <is>
-          <t>Pharmacy</t>
-        </is>
-      </c>
-      <c r="B9" s="4" t="inlineStr">
-        <is>
-          <t>Pharmacy</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>-2.54</v>
-      </c>
-      <c r="D9" t="n">
-        <v>-15.95</v>
-      </c>
-      <c r="E9" t="n">
-        <v>-22.92</v>
-      </c>
-      <c r="F9" t="n">
-        <v>-29.58</v>
-      </c>
-      <c r="G9" t="n">
-        <v>-53.01</v>
-      </c>
-      <c r="H9" t="n">
-        <v>-5.99</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" t="n">
-        <v>-6.99</v>
-      </c>
-      <c r="L9" t="n">
-        <v>-5.84</v>
-      </c>
-      <c r="M9" t="n">
-        <v>-25.06</v>
-      </c>
-      <c r="N9" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" t="n">
-        <v>-167.88</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="4" t="inlineStr">
-        <is>
-          <t>Rent</t>
-        </is>
-      </c>
-      <c r="B10" s="4" t="inlineStr">
-        <is>
-          <t>Rent</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" t="n">
-        <v>0</v>
-      </c>
-      <c r="N10" t="n">
-        <v>0</v>
-      </c>
-      <c r="O10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="4" t="inlineStr">
-        <is>
-          <t>Savings</t>
-        </is>
-      </c>
-      <c r="B11" s="4" t="inlineStr">
-        <is>
-          <t>Savings</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0</v>
-      </c>
-      <c r="K11" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="L11" t="n">
-        <v>-250</v>
-      </c>
-      <c r="M11" t="n">
-        <v>-649.23</v>
-      </c>
-      <c r="N11" t="n">
-        <v>-499.32</v>
-      </c>
-      <c r="O11" t="n">
-        <v>-2398.55</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="4" t="inlineStr">
-        <is>
-          <t>Transportation</t>
-        </is>
-      </c>
-      <c r="B12" s="4" t="inlineStr">
-        <is>
-          <t>Parking</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" t="n">
-        <v>-15</v>
-      </c>
-      <c r="F12" t="n">
-        <v>-4.25</v>
-      </c>
-      <c r="G12" t="n">
-        <v>-4</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0</v>
-      </c>
-      <c r="K12" t="n">
-        <v>0</v>
-      </c>
-      <c r="L12" t="n">
-        <v>0</v>
-      </c>
-      <c r="M12" t="n">
-        <v>0</v>
-      </c>
-      <c r="N12" t="n">
-        <v>0</v>
-      </c>
-      <c r="O12" t="n">
-        <v>-23.25</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="6" t="n"/>
-      <c r="B13" s="4" t="inlineStr">
-        <is>
-          <t>Plane</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" t="n">
-        <v>-150</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" t="n">
-        <v>0</v>
-      </c>
-      <c r="K13" t="n">
-        <v>0</v>
-      </c>
-      <c r="L13" t="n">
-        <v>0</v>
-      </c>
-      <c r="M13" t="n">
-        <v>0</v>
-      </c>
-      <c r="N13" t="n">
-        <v>-30</v>
-      </c>
-      <c r="O13" t="n">
-        <v>-180</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="6" t="n"/>
-      <c r="B14" s="4" t="inlineStr">
-        <is>
-          <t>Rideshare</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" t="n">
-        <v>-31.26</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" t="n">
-        <v>-67.8</v>
-      </c>
-      <c r="G14" t="n">
-        <v>-182.1</v>
-      </c>
-      <c r="H14" t="n">
-        <v>-59.73</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" t="n">
-        <v>0</v>
-      </c>
-      <c r="K14" t="n">
-        <v>-70.12</v>
-      </c>
-      <c r="L14" t="n">
-        <v>0</v>
-      </c>
-      <c r="M14" t="n">
-        <v>0</v>
-      </c>
-      <c r="N14" t="n">
-        <v>0</v>
-      </c>
-      <c r="O14" t="n">
-        <v>-411.01</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="5" t="n"/>
-      <c r="B15" s="4" t="inlineStr">
-        <is>
-          <t>Train</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" t="n">
-        <v>-72</v>
-      </c>
-      <c r="E15" t="n">
-        <v>-31</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0</v>
-      </c>
-      <c r="G15" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" t="n">
-        <v>0</v>
-      </c>
-      <c r="K15" t="n">
-        <v>0</v>
-      </c>
-      <c r="L15" t="n">
-        <v>0</v>
-      </c>
-      <c r="M15" t="n">
-        <v>0</v>
-      </c>
-      <c r="N15" t="n">
-        <v>0</v>
-      </c>
-      <c r="O15" t="n">
-        <v>-103</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A12:A15"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:O15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="4" t="inlineStr">
-        <is>
-          <t>Category</t>
-        </is>
-      </c>
-      <c r="B1" s="4" t="inlineStr">
-        <is>
-          <t>Subcategory</t>
-        </is>
-      </c>
-      <c r="C1" s="4" t="inlineStr">
-        <is>
-          <t>January</t>
-        </is>
-      </c>
-      <c r="D1" s="4" t="inlineStr">
-        <is>
-          <t>February</t>
-        </is>
-      </c>
-      <c r="E1" s="4" t="inlineStr">
-        <is>
-          <t>March</t>
-        </is>
-      </c>
-      <c r="F1" s="4" t="inlineStr">
-        <is>
-          <t>April</t>
-        </is>
-      </c>
-      <c r="G1" s="4" t="inlineStr">
-        <is>
-          <t>May</t>
-        </is>
-      </c>
-      <c r="H1" s="4" t="inlineStr">
-        <is>
-          <t>June</t>
-        </is>
-      </c>
-      <c r="I1" s="4" t="inlineStr">
-        <is>
-          <t>July</t>
-        </is>
-      </c>
-      <c r="J1" s="4" t="inlineStr">
-        <is>
-          <t>August</t>
-        </is>
-      </c>
-      <c r="K1" s="4" t="inlineStr">
-        <is>
-          <t>September</t>
-        </is>
-      </c>
-      <c r="L1" s="4" t="inlineStr">
-        <is>
-          <t>October</t>
-        </is>
-      </c>
-      <c r="M1" s="4" t="inlineStr">
-        <is>
-          <t>November</t>
-        </is>
-      </c>
-      <c r="N1" s="4" t="inlineStr">
-        <is>
-          <t>December</t>
-        </is>
-      </c>
-      <c r="O1" s="4" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="inlineStr">
-        <is>
-          <t>Drink</t>
-        </is>
-      </c>
-      <c r="B2" s="4" t="inlineStr">
-        <is>
-          <t>Bar</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>-39.53</v>
-      </c>
-      <c r="F2" t="n">
-        <v>-37.69</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>-36.58</v>
-      </c>
-      <c r="I2" t="n">
-        <v>-23.2</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" t="n">
-        <v>-52.1</v>
-      </c>
-      <c r="L2" t="n">
-        <v>-30.94</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" t="n">
-        <v>-220.04</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="5" t="n"/>
-      <c r="B3" s="4" t="inlineStr">
-        <is>
-          <t>Counter</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>-44.16</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>-60.93</v>
-      </c>
-      <c r="F3" t="n">
-        <v>-24</v>
-      </c>
-      <c r="G3" t="n">
-        <v>-69.73</v>
-      </c>
-      <c r="H3" t="n">
-        <v>-44.56999999999999</v>
-      </c>
-      <c r="I3" t="n">
-        <v>-28.27</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" t="n">
-        <v>-3.54</v>
-      </c>
-      <c r="L3" t="n">
-        <v>-48.43</v>
-      </c>
-      <c r="M3" t="n">
-        <v>-11.84</v>
-      </c>
-      <c r="N3" t="n">
-        <v>-4.35</v>
-      </c>
-      <c r="O3" t="n">
-        <v>-339.82</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="inlineStr">
-        <is>
-          <t>Food</t>
-        </is>
-      </c>
-      <c r="B4" s="4" t="inlineStr">
-        <is>
-          <t>Groceries</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>-6.67</v>
-      </c>
-      <c r="D4" t="n">
-        <v>-14.48</v>
-      </c>
-      <c r="E4" t="n">
-        <v>-61.58</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>-20.82</v>
-      </c>
-      <c r="H4" t="n">
-        <v>-68.91</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" t="n">
-        <v>-7.42</v>
-      </c>
-      <c r="L4" t="n">
-        <v>-2.49</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" t="n">
-        <v>-15.99</v>
-      </c>
-      <c r="O4" t="n">
-        <v>-198.36</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="n"/>
-      <c r="B5" s="4" t="inlineStr">
-        <is>
-          <t>Restaurant</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>-54.54</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-19.77</v>
-      </c>
-      <c r="E5" t="n">
-        <v>-19.07</v>
-      </c>
-      <c r="F5" t="n">
-        <v>-56.84999999999999</v>
-      </c>
-      <c r="G5" t="n">
-        <v>-188.11</v>
-      </c>
-      <c r="H5" t="n">
-        <v>-124.51</v>
-      </c>
-      <c r="I5" t="n">
-        <v>-66.7</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" t="n">
-        <v>-109.59</v>
-      </c>
-      <c r="L5" t="n">
-        <v>-80.69</v>
-      </c>
-      <c r="M5" t="n">
-        <v>-68.73</v>
-      </c>
-      <c r="N5" t="n">
-        <v>-63.09</v>
-      </c>
-      <c r="O5" t="n">
-        <v>-851.6500000000002</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="inlineStr">
-        <is>
-          <t>Income</t>
-        </is>
-      </c>
-      <c r="B6" s="4" t="inlineStr">
-        <is>
-          <t>Tutoring</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L6" t="n">
-        <v>348.44</v>
-      </c>
-      <c r="M6" t="n">
-        <v>962.03</v>
-      </c>
-      <c r="N6" t="n">
-        <v>694.49</v>
-      </c>
-      <c r="O6" t="n">
-        <v>2004.96</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="inlineStr">
-        <is>
-          <t>Miscellaneous</t>
-        </is>
-      </c>
-      <c r="B7" s="4" t="inlineStr">
-        <is>
-          <t>Bank</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>-199.67</v>
-      </c>
-      <c r="D7" t="n">
-        <v>-19.86</v>
-      </c>
-      <c r="E7" t="n">
-        <v>-18.92</v>
-      </c>
-      <c r="F7" t="n">
-        <v>-58.89</v>
-      </c>
-      <c r="G7" t="n">
-        <v>-38.91</v>
-      </c>
-      <c r="H7" t="n">
-        <v>-79.24000000000001</v>
-      </c>
-      <c r="I7" t="n">
-        <v>-59.25</v>
-      </c>
-      <c r="J7" t="n">
-        <v>-39.24</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="M7" t="n">
-        <v>-59.9</v>
-      </c>
-      <c r="N7" t="n">
-        <v>0</v>
-      </c>
-      <c r="O7" t="n">
-        <v>-573.4400000000001</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="5" t="n"/>
-      <c r="B8" s="4" t="inlineStr">
-        <is>
-          <t>Miscellaneous</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>-106.48</v>
-      </c>
-      <c r="D8" t="n">
-        <v>-74.8</v>
-      </c>
-      <c r="E8" t="n">
-        <v>3476.46</v>
-      </c>
-      <c r="F8" t="n">
-        <v>-146.88</v>
-      </c>
-      <c r="G8" t="n">
-        <v>-173.02</v>
-      </c>
-      <c r="H8" t="n">
-        <v>94.92</v>
-      </c>
-      <c r="I8" t="n">
-        <v>349.8</v>
-      </c>
-      <c r="J8" t="n">
-        <v>-66.71000000000001</v>
-      </c>
-      <c r="K8" t="n">
-        <v>-187.81</v>
-      </c>
-      <c r="L8" t="n">
-        <v>-57.46000000000001</v>
-      </c>
-      <c r="M8" t="n">
-        <v>-234.09</v>
-      </c>
-      <c r="N8" t="n">
-        <v>-166.94</v>
-      </c>
-      <c r="O8" t="n">
-        <v>2706.99</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="4" t="inlineStr">
-        <is>
-          <t>Pharmacy</t>
-        </is>
-      </c>
-      <c r="B9" s="4" t="inlineStr">
-        <is>
-          <t>Pharmacy</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>-2.54</v>
-      </c>
-      <c r="D9" t="n">
-        <v>-15.95</v>
-      </c>
-      <c r="E9" t="n">
-        <v>-22.92</v>
-      </c>
-      <c r="F9" t="n">
-        <v>-29.58</v>
-      </c>
-      <c r="G9" t="n">
-        <v>-53.01</v>
-      </c>
-      <c r="H9" t="n">
-        <v>-5.99</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" t="n">
-        <v>-6.99</v>
-      </c>
-      <c r="L9" t="n">
-        <v>-5.84</v>
-      </c>
-      <c r="M9" t="n">
-        <v>-25.06</v>
-      </c>
-      <c r="N9" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" t="n">
-        <v>-167.88</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="4" t="inlineStr">
-        <is>
-          <t>Rent</t>
-        </is>
-      </c>
-      <c r="B10" s="4" t="inlineStr">
-        <is>
-          <t>Rent</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" t="n">
-        <v>0</v>
-      </c>
-      <c r="N10" t="n">
-        <v>0</v>
-      </c>
-      <c r="O10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="4" t="inlineStr">
-        <is>
-          <t>Savings</t>
-        </is>
-      </c>
-      <c r="B11" s="4" t="inlineStr">
-        <is>
-          <t>Savings</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0</v>
-      </c>
-      <c r="K11" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="L11" t="n">
-        <v>-250</v>
-      </c>
-      <c r="M11" t="n">
-        <v>-649.23</v>
-      </c>
-      <c r="N11" t="n">
-        <v>-499.32</v>
-      </c>
-      <c r="O11" t="n">
-        <v>-2398.55</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="4" t="inlineStr">
-        <is>
-          <t>Transportation</t>
-        </is>
-      </c>
-      <c r="B12" s="4" t="inlineStr">
-        <is>
-          <t>Parking</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" t="n">
-        <v>-15</v>
-      </c>
-      <c r="F12" t="n">
-        <v>-4.25</v>
-      </c>
-      <c r="G12" t="n">
-        <v>-4</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0</v>
-      </c>
-      <c r="K12" t="n">
-        <v>0</v>
-      </c>
-      <c r="L12" t="n">
-        <v>0</v>
-      </c>
-      <c r="M12" t="n">
-        <v>0</v>
-      </c>
-      <c r="N12" t="n">
-        <v>0</v>
-      </c>
-      <c r="O12" t="n">
-        <v>-23.25</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="6" t="n"/>
-      <c r="B13" s="4" t="inlineStr">
-        <is>
-          <t>Plane</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" t="n">
-        <v>-150</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" t="n">
-        <v>0</v>
-      </c>
-      <c r="K13" t="n">
-        <v>0</v>
-      </c>
-      <c r="L13" t="n">
-        <v>0</v>
-      </c>
-      <c r="M13" t="n">
-        <v>0</v>
-      </c>
-      <c r="N13" t="n">
-        <v>-30</v>
-      </c>
-      <c r="O13" t="n">
-        <v>-180</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="6" t="n"/>
-      <c r="B14" s="4" t="inlineStr">
-        <is>
-          <t>Rideshare</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" t="n">
-        <v>-31.26</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" t="n">
-        <v>-67.8</v>
-      </c>
-      <c r="G14" t="n">
-        <v>-182.1</v>
-      </c>
-      <c r="H14" t="n">
-        <v>-59.73</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" t="n">
-        <v>0</v>
-      </c>
-      <c r="K14" t="n">
-        <v>-70.12</v>
-      </c>
-      <c r="L14" t="n">
-        <v>0</v>
-      </c>
-      <c r="M14" t="n">
-        <v>0</v>
-      </c>
-      <c r="N14" t="n">
-        <v>0</v>
-      </c>
-      <c r="O14" t="n">
-        <v>-411.01</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="5" t="n"/>
-      <c r="B15" s="4" t="inlineStr">
-        <is>
-          <t>Train</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" t="n">
-        <v>-72</v>
-      </c>
-      <c r="E15" t="n">
-        <v>-31</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0</v>
-      </c>
-      <c r="G15" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" t="n">
-        <v>0</v>
-      </c>
-      <c r="K15" t="n">
-        <v>0</v>
-      </c>
-      <c r="L15" t="n">
-        <v>0</v>
-      </c>
-      <c r="M15" t="n">
-        <v>0</v>
-      </c>
-      <c r="N15" t="n">
-        <v>0</v>
-      </c>
-      <c r="O15" t="n">
-        <v>-103</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A12:A15"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:O15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="4" t="inlineStr">
-        <is>
-          <t>Category</t>
-        </is>
-      </c>
-      <c r="B1" s="4" t="inlineStr">
-        <is>
-          <t>Subcategory</t>
-        </is>
-      </c>
-      <c r="C1" s="4" t="inlineStr">
-        <is>
-          <t>January</t>
-        </is>
-      </c>
-      <c r="D1" s="4" t="inlineStr">
-        <is>
-          <t>February</t>
-        </is>
-      </c>
-      <c r="E1" s="4" t="inlineStr">
-        <is>
-          <t>March</t>
-        </is>
-      </c>
-      <c r="F1" s="4" t="inlineStr">
-        <is>
-          <t>April</t>
-        </is>
-      </c>
-      <c r="G1" s="4" t="inlineStr">
-        <is>
-          <t>May</t>
-        </is>
-      </c>
-      <c r="H1" s="4" t="inlineStr">
-        <is>
-          <t>June</t>
-        </is>
-      </c>
-      <c r="I1" s="4" t="inlineStr">
-        <is>
-          <t>July</t>
-        </is>
-      </c>
-      <c r="J1" s="4" t="inlineStr">
-        <is>
-          <t>August</t>
-        </is>
-      </c>
-      <c r="K1" s="4" t="inlineStr">
-        <is>
-          <t>September</t>
-        </is>
-      </c>
-      <c r="L1" s="4" t="inlineStr">
-        <is>
-          <t>October</t>
-        </is>
-      </c>
-      <c r="M1" s="4" t="inlineStr">
-        <is>
-          <t>November</t>
-        </is>
-      </c>
-      <c r="N1" s="4" t="inlineStr">
-        <is>
-          <t>December</t>
-        </is>
-      </c>
-      <c r="O1" s="4" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="inlineStr">
-        <is>
-          <t>Drink</t>
-        </is>
-      </c>
-      <c r="B2" s="4" t="inlineStr">
-        <is>
-          <t>Bar</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>-39.53</v>
-      </c>
-      <c r="F2" t="n">
-        <v>-37.69</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>-36.58</v>
-      </c>
-      <c r="I2" t="n">
-        <v>-23.2</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" t="n">
-        <v>-52.1</v>
-      </c>
-      <c r="L2" t="n">
-        <v>-30.94</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" t="n">
-        <v>-220.04</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="5" t="n"/>
-      <c r="B3" s="4" t="inlineStr">
-        <is>
-          <t>Counter</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>-44.16</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>-60.93</v>
-      </c>
-      <c r="F3" t="n">
-        <v>-24</v>
-      </c>
-      <c r="G3" t="n">
-        <v>-69.73</v>
-      </c>
-      <c r="H3" t="n">
-        <v>-44.56999999999999</v>
-      </c>
-      <c r="I3" t="n">
-        <v>-28.27</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" t="n">
-        <v>-3.54</v>
-      </c>
-      <c r="L3" t="n">
-        <v>-48.43</v>
-      </c>
-      <c r="M3" t="n">
-        <v>-11.84</v>
-      </c>
-      <c r="N3" t="n">
-        <v>-4.35</v>
-      </c>
-      <c r="O3" t="n">
-        <v>-339.82</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="inlineStr">
-        <is>
-          <t>Food</t>
-        </is>
-      </c>
-      <c r="B4" s="4" t="inlineStr">
-        <is>
-          <t>Groceries</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>-6.67</v>
-      </c>
-      <c r="D4" t="n">
-        <v>-14.48</v>
-      </c>
-      <c r="E4" t="n">
-        <v>-61.58</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>-20.82</v>
-      </c>
-      <c r="H4" t="n">
-        <v>-68.91</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" t="n">
-        <v>-7.42</v>
-      </c>
-      <c r="L4" t="n">
-        <v>-2.49</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" t="n">
-        <v>-15.99</v>
-      </c>
-      <c r="O4" t="n">
-        <v>-198.36</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5" t="n"/>
-      <c r="B5" s="4" t="inlineStr">
-        <is>
-          <t>Restaurant</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>-54.54</v>
-      </c>
-      <c r="D5" t="n">
-        <v>-19.77</v>
-      </c>
-      <c r="E5" t="n">
-        <v>-19.07</v>
-      </c>
-      <c r="F5" t="n">
-        <v>-56.84999999999999</v>
-      </c>
-      <c r="G5" t="n">
-        <v>-188.11</v>
-      </c>
-      <c r="H5" t="n">
-        <v>-124.51</v>
-      </c>
-      <c r="I5" t="n">
-        <v>-66.7</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" t="n">
-        <v>-109.59</v>
-      </c>
-      <c r="L5" t="n">
-        <v>-80.69</v>
-      </c>
-      <c r="M5" t="n">
-        <v>-68.73</v>
-      </c>
-      <c r="N5" t="n">
-        <v>-63.09</v>
-      </c>
-      <c r="O5" t="n">
-        <v>-851.6500000000002</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="inlineStr">
-        <is>
-          <t>Income</t>
-        </is>
-      </c>
-      <c r="B6" s="4" t="inlineStr">
-        <is>
-          <t>Tutoring</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0</v>
-      </c>
-      <c r="L6" t="n">
-        <v>348.44</v>
-      </c>
-      <c r="M6" t="n">
-        <v>962.03</v>
-      </c>
-      <c r="N6" t="n">
-        <v>694.49</v>
-      </c>
-      <c r="O6" t="n">
-        <v>2004.96</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="inlineStr">
-        <is>
-          <t>Miscellaneous</t>
-        </is>
-      </c>
-      <c r="B7" s="4" t="inlineStr">
-        <is>
-          <t>Bank</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>-199.67</v>
-      </c>
-      <c r="D7" t="n">
-        <v>-19.86</v>
-      </c>
-      <c r="E7" t="n">
-        <v>-18.92</v>
-      </c>
-      <c r="F7" t="n">
-        <v>-58.89</v>
-      </c>
-      <c r="G7" t="n">
-        <v>-38.91</v>
-      </c>
-      <c r="H7" t="n">
-        <v>-79.24000000000001</v>
-      </c>
-      <c r="I7" t="n">
-        <v>-59.25</v>
-      </c>
-      <c r="J7" t="n">
-        <v>-39.24</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="M7" t="n">
-        <v>-59.9</v>
-      </c>
-      <c r="N7" t="n">
-        <v>0</v>
-      </c>
-      <c r="O7" t="n">
-        <v>-573.4400000000001</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="5" t="n"/>
-      <c r="B8" s="4" t="inlineStr">
-        <is>
-          <t>Miscellaneous</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>-106.48</v>
-      </c>
-      <c r="D8" t="n">
-        <v>-74.8</v>
-      </c>
-      <c r="E8" t="n">
-        <v>3476.46</v>
-      </c>
-      <c r="F8" t="n">
-        <v>-146.88</v>
-      </c>
-      <c r="G8" t="n">
-        <v>-173.02</v>
-      </c>
-      <c r="H8" t="n">
-        <v>94.92</v>
-      </c>
-      <c r="I8" t="n">
-        <v>349.8</v>
-      </c>
-      <c r="J8" t="n">
-        <v>-66.71000000000001</v>
-      </c>
-      <c r="K8" t="n">
-        <v>-187.81</v>
-      </c>
-      <c r="L8" t="n">
-        <v>-57.46000000000001</v>
-      </c>
-      <c r="M8" t="n">
-        <v>-234.09</v>
-      </c>
-      <c r="N8" t="n">
-        <v>-166.94</v>
-      </c>
-      <c r="O8" t="n">
-        <v>2706.99</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="4" t="inlineStr">
-        <is>
-          <t>Pharmacy</t>
-        </is>
-      </c>
-      <c r="B9" s="4" t="inlineStr">
-        <is>
-          <t>Pharmacy</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>-2.54</v>
-      </c>
-      <c r="D9" t="n">
-        <v>-15.95</v>
-      </c>
-      <c r="E9" t="n">
-        <v>-22.92</v>
-      </c>
-      <c r="F9" t="n">
-        <v>-29.58</v>
-      </c>
-      <c r="G9" t="n">
-        <v>-53.01</v>
-      </c>
-      <c r="H9" t="n">
-        <v>-5.99</v>
-      </c>
-      <c r="I9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" t="n">
-        <v>-6.99</v>
-      </c>
-      <c r="L9" t="n">
-        <v>-5.84</v>
-      </c>
-      <c r="M9" t="n">
-        <v>-25.06</v>
-      </c>
-      <c r="N9" t="n">
-        <v>0</v>
-      </c>
-      <c r="O9" t="n">
-        <v>-167.88</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="4" t="inlineStr">
-        <is>
-          <t>Rent</t>
-        </is>
-      </c>
-      <c r="B10" s="4" t="inlineStr">
-        <is>
-          <t>Rent</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" t="n">
-        <v>0</v>
-      </c>
-      <c r="N10" t="n">
-        <v>0</v>
-      </c>
-      <c r="O10" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="4" t="inlineStr">
-        <is>
-          <t>Savings</t>
-        </is>
-      </c>
-      <c r="B11" s="4" t="inlineStr">
-        <is>
-          <t>Savings</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" t="n">
-        <v>0</v>
-      </c>
-      <c r="G11" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0</v>
-      </c>
-      <c r="K11" t="n">
-        <v>-1000</v>
-      </c>
-      <c r="L11" t="n">
-        <v>-250</v>
-      </c>
-      <c r="M11" t="n">
-        <v>-649.23</v>
-      </c>
-      <c r="N11" t="n">
-        <v>-499.32</v>
-      </c>
-      <c r="O11" t="n">
-        <v>-2398.55</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="4" t="inlineStr">
-        <is>
-          <t>Transportation</t>
-        </is>
-      </c>
-      <c r="B12" s="4" t="inlineStr">
-        <is>
-          <t>Parking</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" t="n">
-        <v>-15</v>
-      </c>
-      <c r="F12" t="n">
-        <v>-4.25</v>
-      </c>
-      <c r="G12" t="n">
-        <v>-4</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0</v>
-      </c>
-      <c r="K12" t="n">
-        <v>0</v>
-      </c>
-      <c r="L12" t="n">
-        <v>0</v>
-      </c>
-      <c r="M12" t="n">
-        <v>0</v>
-      </c>
-      <c r="N12" t="n">
-        <v>0</v>
-      </c>
-      <c r="O12" t="n">
-        <v>-23.25</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="6" t="n"/>
-      <c r="B13" s="4" t="inlineStr">
-        <is>
-          <t>Plane</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" t="n">
-        <v>-150</v>
-      </c>
-      <c r="I13" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" t="n">
-        <v>0</v>
-      </c>
-      <c r="K13" t="n">
-        <v>0</v>
-      </c>
-      <c r="L13" t="n">
-        <v>0</v>
-      </c>
-      <c r="M13" t="n">
-        <v>0</v>
-      </c>
-      <c r="N13" t="n">
-        <v>-30</v>
-      </c>
-      <c r="O13" t="n">
-        <v>-180</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="6" t="n"/>
-      <c r="B14" s="4" t="inlineStr">
-        <is>
-          <t>Rideshare</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" t="n">
-        <v>-31.26</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" t="n">
-        <v>-67.8</v>
-      </c>
-      <c r="G14" t="n">
-        <v>-182.1</v>
-      </c>
-      <c r="H14" t="n">
-        <v>-59.73</v>
-      </c>
-      <c r="I14" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" t="n">
-        <v>0</v>
-      </c>
-      <c r="K14" t="n">
-        <v>-70.12</v>
-      </c>
-      <c r="L14" t="n">
-        <v>0</v>
-      </c>
-      <c r="M14" t="n">
-        <v>0</v>
-      </c>
-      <c r="N14" t="n">
-        <v>0</v>
-      </c>
-      <c r="O14" t="n">
-        <v>-411.01</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="5" t="n"/>
-      <c r="B15" s="4" t="inlineStr">
-        <is>
-          <t>Train</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" t="n">
-        <v>-72</v>
-      </c>
-      <c r="E15" t="n">
-        <v>-31</v>
-      </c>
-      <c r="F15" t="n">
-        <v>0</v>
-      </c>
-      <c r="G15" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" t="n">
-        <v>0</v>
-      </c>
-      <c r="K15" t="n">
-        <v>0</v>
-      </c>
-      <c r="L15" t="n">
-        <v>0</v>
-      </c>
-      <c r="M15" t="n">
-        <v>0</v>
-      </c>
-      <c r="N15" t="n">
-        <v>0</v>
-      </c>
-      <c r="O15" t="n">
-        <v>-103</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="A12:A15"/>
-  </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:O15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="4" t="inlineStr">
-        <is>
-          <t>Category</t>
-        </is>
-      </c>
-      <c r="B1" s="4" t="inlineStr">
-        <is>
-          <t>Subcategory</t>
-        </is>
-      </c>
-      <c r="C1" s="4" t="inlineStr">
-        <is>
-          <t>January</t>
-        </is>
-      </c>
-      <c r="D1" s="4" t="inlineStr">
-        <is>
-          <t>February</t>
-        </is>
-      </c>
-      <c r="E1" s="4" t="inlineStr">
-        <is>
-          <t>March</t>
-        </is>
-      </c>
-      <c r="F1" s="4" t="inlineStr">
-        <is>
-          <t>April</t>
-        </is>
-      </c>
-      <c r="G1" s="4" t="inlineStr">
-        <is>
-          <t>May</t>
-        </is>
-      </c>
-      <c r="H1" s="4" t="inlineStr">
-        <is>
-          <t>June</t>
-        </is>
-      </c>
-      <c r="I1" s="4" t="inlineStr">
-        <is>
-          <t>July</t>
-        </is>
-      </c>
-      <c r="J1" s="4" t="inlineStr">
-        <is>
-          <t>August</t>
-        </is>
-      </c>
-      <c r="K1" s="4" t="inlineStr">
-        <is>
-          <t>September</t>
-        </is>
-      </c>
-      <c r="L1" s="4" t="inlineStr">
-        <is>
-          <t>October</t>
-        </is>
-      </c>
-      <c r="M1" s="4" t="inlineStr">
-        <is>
-          <t>November</t>
-        </is>
-      </c>
-      <c r="N1" s="4" t="inlineStr">
-        <is>
-          <t>December</t>
-        </is>
-      </c>
-      <c r="O1" s="4" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="inlineStr">
-        <is>
-          <t>Drink</t>
-        </is>
-      </c>
-      <c r="B2" s="4" t="inlineStr">
-        <is>
-          <t>Bar</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>-39.53</v>
-      </c>
-      <c r="F2" t="n">
-        <v>-37.69</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H2" t="n">
-        <v>-36.58</v>
-      </c>
-      <c r="I2" t="n">
-        <v>-23.2</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" t="n">
-        <v>-52.1</v>
-      </c>
-      <c r="L2" t="n">
-        <v>-30.94</v>
-      </c>
-      <c r="M2" t="n">
-        <v>0</v>
-      </c>
-      <c r="N2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" t="n">
-        <v>-220.04</v>
-      </c>
-    </row>
-    <row r="3">
       <c r="A3" s="4" t="n"/>
       <c r="B3" s="4" t="inlineStr">
         <is>

</xml_diff>